<commit_message>
adding samples for outputs
</commit_message>
<xml_diff>
--- a/oci-list-resources/examples/example_oci_resources_frvkqml7frsy_2025-10-29.xlsx
+++ b/oci-list-resources/examples/example_oci_resources_frvkqml7frsy_2025-10-29.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geconsta/work/oci-list-resources-python/oci-list-resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geconsta/work/oci-list-resources-python/oci-list-resources/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F991858-2164-EC44-98DC-29724D6998EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF1B9BE-6AEF-4E44-BCE0-96FC3F569AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="760" windowWidth="28700" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,9 +189,6 @@
     <t>ocid1.instance.oc1.eu-frankfurt-1.antheljro7vto7ic2ebjmpgnijbj7v7gujtehtpxloqir24jxnt6wznlb7oq</t>
   </si>
   <si>
-    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/marius.ciotir@oracle.com', 'CreatedOn': '2025-07-25T17:18:09.781Z'}}</t>
-  </si>
-  <si>
     <t>{'isv_labs': '0.0.1', 'Managedby': 'Terraform'}</t>
   </si>
   <si>
@@ -201,27 +198,18 @@
     <t>ocid1.instance.oc1.eu-frankfurt-1.antheljro7vto7ici53keqpbxobz44xg2iage466hn5or5wsslqe57isblka</t>
   </si>
   <si>
-    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/marius.ciotir@oracle.com', 'CreatedOn': '2025-10-24T09:15:42.852Z'}}</t>
-  </si>
-  <si>
     <t>instance-20251028-1951</t>
   </si>
   <si>
     <t>ocid1.instance.oc1.eu-frankfurt-1.antheljro7vto7icjailxaiva3m3buslskc2qznbhyrgltgou3tictdikv6q</t>
   </si>
   <si>
-    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/marius.ciotir@oracle.com', 'CreatedOn': '2025-10-28T17:54:24.461Z'}}</t>
-  </si>
-  <si>
     <t>jenkis</t>
   </si>
   <si>
     <t>ocid1.instance.oc1.eu-frankfurt-1.antheljro7vto7icltmwvql5odk4loa4lbc65lvb3pci6v57lx74ylxx6hoa</t>
   </si>
   <si>
-    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/marius.ciotir@oracle.com', 'CreatedOn': '2025-10-23T12:05:43.000Z'}}</t>
-  </si>
-  <si>
     <t>csi-3e0d5a22-0d02-4ea1-aab5-4bc25749373e</t>
   </si>
   <si>
@@ -357,45 +345,30 @@
     <t>ocid1.filesystem.oc1.eu_frankfurt_1.aaaaaaaaaalwn2vbmzzgcllqojxwiotfouwwm4tbnzvwm5lsoqwtcllbmqwtcaaa</t>
   </si>
   <si>
-    <t>{'Oracle-Tags': {'CreatedBy': 'default/bogdan.m.darie@oracle.com', 'CreatedOn': '2025-07-15T09:25:04.364Z'}}</t>
-  </si>
-  <si>
     <t>RAGATP23</t>
   </si>
   <si>
     <t>ocid1.autonomousdatabase.oc1.eu-frankfurt-1.antheljro7vto7ia7lbw5wqs5hml2hlgcouoxco54t34xqfwms5obu7s5q4a</t>
   </si>
   <si>
-    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/george.soare@oracle.com', 'CreatedOn': '2025-10-18T10:31:36.824Z'}}</t>
-  </si>
-  <si>
     <t>RAG_WITH_RAS</t>
   </si>
   <si>
     <t>ocid1.autonomousdatabase.oc1.eu-frankfurt-1.antheljto7vto7iabaf5ffyq3l66u6bkduajim47ukumr64poutrvt7pzc5q</t>
   </si>
   <si>
-    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/george.soare@oracle.com', 'CreatedOn': '2025-10-27T07:41:20.526Z'}}</t>
-  </si>
-  <si>
     <t>RAG_DB_USERS</t>
   </si>
   <si>
     <t>ocid1.autonomousdatabase.oc1.eu-frankfurt-1.antheljto7vto7iamj67l2ynd45otjsjq3guazerzon3lknbbu5heloe2cjq</t>
   </si>
   <si>
-    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/george.soare@oracle.com', 'CreatedOn': '2025-10-20T12:12:39.569Z'}}</t>
-  </si>
-  <si>
     <t>RAGDB_APEX</t>
   </si>
   <si>
     <t>ocid1.autonomousdatabase.oc1.eu-frankfurt-1.antheljto7vto7iavldtwfl4f6mktf52zw2sy64s6xyh26abot5ln44vb7jq</t>
   </si>
   <si>
-    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/george.soare@oracle.com', 'CreatedOn': '2025-10-20T12:15:01.708Z'}}</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
@@ -409,6 +382,33 @@
   </si>
   <si>
     <t>Autonomous Databases</t>
+  </si>
+  <si>
+    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/xxxx.xxxx@oracle.com', 'CreatedOn': '2025-07-25T17:18:09.781Z'}}</t>
+  </si>
+  <si>
+    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/xxxx.xxxx@oracle.com', 'CreatedOn': '2025-10-24T09:15:42.852Z'}}</t>
+  </si>
+  <si>
+    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/xxxx.xxxx@oracle.com', 'CreatedOn': '2025-10-28T17:54:24.461Z'}}</t>
+  </si>
+  <si>
+    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/xxxx.xxxx@oracle.com', 'CreatedOn': '2025-10-23T12:05:43.000Z'}}</t>
+  </si>
+  <si>
+    <t>{'Oracle-Tags': {'CreatedBy': 'default/xxxx.xxxx@oracle.com', 'CreatedOn': '2025-07-15T09:25:04.364Z'}}</t>
+  </si>
+  <si>
+    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/xxxx.xxxx@oracle.com', 'CreatedOn': '2025-10-18T10:31:36.824Z'}}</t>
+  </si>
+  <si>
+    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/xxxx.xxxx@oracle.com', 'CreatedOn': '2025-10-27T07:41:20.526Z'}}</t>
+  </si>
+  <si>
+    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/xxxx.xxxx@oracle.com', 'CreatedOn': '2025-10-20T12:12:39.569Z'}}</t>
+  </si>
+  <si>
+    <t>{'Do-not-stop-scheduler': {'Stop': 'FALSE'}, 'Oracle-Tags': {'CreatedBy': 'default/xxxx.xxxx@oracle.com', 'CreatedOn': '2025-10-20T12:15:01.708Z'}}</t>
   </si>
 </sst>
 </file>
@@ -1684,7 +1684,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1723,10 +1725,10 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" t="s">
         <v>54</v>
-      </c>
-      <c r="E2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1734,16 +1736,16 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1751,13 +1753,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="E4" t="s">
         <v>51</v>
@@ -1768,16 +1770,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1792,7 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -1802,6 +1804,7 @@
     <col min="2" max="2" width="59.83203125" customWidth="1"/>
     <col min="3" max="3" width="85.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="168.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1826,16 +1829,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1843,16 +1846,16 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1860,16 +1863,16 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1877,16 +1880,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1894,16 +1897,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1911,16 +1914,16 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1928,16 +1931,16 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1945,13 +1948,13 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E9" t="s">
         <v>51</v>
@@ -1962,13 +1965,13 @@
         <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E10" t="s">
         <v>51</v>
@@ -1979,13 +1982,13 @@
         <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E11" t="s">
         <v>51</v>
@@ -1996,13 +1999,13 @@
         <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E12" t="s">
         <v>51</v>
@@ -2013,13 +2016,13 @@
         <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E13" t="s">
         <v>51</v>
@@ -2030,13 +2033,13 @@
         <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
         <v>51</v>
@@ -2054,7 +2057,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2087,13 +2092,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
         <v>51</v>
@@ -2104,13 +2109,13 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="E3" t="s">
         <v>51</v>
@@ -2129,7 +2134,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2137,8 +2142,8 @@
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="94.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="186.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="111.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2163,13 +2168,13 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s">
         <v>51</v>
@@ -2180,13 +2185,13 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="E3" t="s">
         <v>51</v>
@@ -2197,13 +2202,13 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
         <v>51</v>
@@ -2214,13 +2219,13 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>
@@ -2239,7 +2244,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2252,12 +2257,12 @@
         <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B2">
         <v>235</v>
@@ -2265,7 +2270,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B3">
         <v>85</v>
@@ -2273,7 +2278,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -2281,7 +2286,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B5">
         <v>27</v>

</xml_diff>